<commit_message>
Update 'Grenseverdier fra Sylvia'
</commit_message>
<xml_diff>
--- a/Input_data/Grenseverdier_fra_Sylvia.xlsx
+++ b/Input_data/Grenseverdier_fra_Sylvia.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17030"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\niva-of5\osl-userdata$\DHJ\Documents\seksjon 212\Indikator 2018\Data NIFES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\seksjon 212\Contaminant_indicators\Input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1CD232-7CA7-4E23-AFE0-35EFB4861DDA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22050" windowHeight="9540"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22050" windowHeight="9540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="for R" sheetId="3" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="44">
   <si>
     <t>Miljøgift</t>
   </si>
@@ -148,12 +149,21 @@
   </si>
   <si>
     <t>PARAM</t>
+  </si>
+  <si>
+    <t>CB_S7</t>
+  </si>
+  <si>
+    <t>DDEPP</t>
+  </si>
+  <si>
+    <t>BDE6S</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -507,371 +517,392 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="4" width="20.85546875" customWidth="1"/>
+    <col min="1" max="2" width="39.7109375" customWidth="1"/>
+    <col min="3" max="3" width="43" customWidth="1"/>
+    <col min="4" max="5" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>33</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>34</v>
       </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
       <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="G2">
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2">
         <v>20</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>35</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>33</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>37</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>33</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>34</v>
       </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5">
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6">
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>35</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>36</v>
       </c>
-      <c r="F7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7">
+      <c r="G7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>33</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>34</v>
       </c>
-      <c r="E8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8">
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>35</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>36</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
         <v>6</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>33</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>34</v>
-      </c>
-      <c r="G11">
-        <v>3.5000000000000001E-3</v>
       </c>
       <c r="H11">
         <v>3.5000000000000001E-3</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="J11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
         <v>6</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>35</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>36</v>
       </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="G12">
-        <v>3.5000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="H12">
         <v>3.5000000000000001E-3</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="J12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
         <v>6</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>33</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>34</v>
-      </c>
-      <c r="G13">
-        <v>6.4999999999999997E-3</v>
       </c>
       <c r="H13">
         <v>6.4999999999999997E-3</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="J13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
         <v>6</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>35</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>36</v>
       </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
       <c r="F14">
         <v>0</v>
       </c>
       <c r="G14">
-        <v>6.4999999999999997E-3</v>
+        <v>0</v>
       </c>
       <c r="H14">
         <v>6.4999999999999997E-3</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="J14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
         <v>8</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>33</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>37</v>
       </c>
-      <c r="E15" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15">
-        <v>6.4999999999999997E-3</v>
+      <c r="F15" t="s">
+        <v>7</v>
       </c>
       <c r="H15">
         <v>6.4999999999999997E-3</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="J15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>6</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>33</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>34</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>6</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>35</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>36</v>
       </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
       <c r="F17">
         <v>0</v>
       </c>
@@ -879,439 +910,481 @@
         <v>0</v>
       </c>
       <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
         <v>75</v>
       </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
         <v>15</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>8</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>33</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>37</v>
       </c>
-      <c r="E18" t="s">
-        <v>7</v>
-      </c>
       <c r="F18" t="s">
         <v>7</v>
       </c>
-      <c r="H18">
+      <c r="G18" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18">
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
-      <c r="B19" t="s">
-        <v>17</v>
-      </c>
       <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" t="s">
         <v>33</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>37</v>
       </c>
-      <c r="E19" t="s">
-        <v>7</v>
-      </c>
       <c r="F19" t="s">
         <v>7</v>
       </c>
-      <c r="G19">
+      <c r="G19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19">
         <v>10</v>
       </c>
-      <c r="H19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
-      <c r="B20" t="s">
-        <v>17</v>
-      </c>
       <c r="C20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" t="s">
         <v>35</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>36</v>
       </c>
-      <c r="E20" t="s">
-        <v>7</v>
-      </c>
       <c r="F20" t="s">
         <v>7</v>
       </c>
-      <c r="G20">
+      <c r="G20" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20">
         <v>10</v>
       </c>
-      <c r="H20" t="s">
-        <v>26</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>26</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
         <v>18</v>
       </c>
-      <c r="B21" t="s">
-        <v>17</v>
-      </c>
       <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" t="s">
         <v>33</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>37</v>
       </c>
-      <c r="E21" t="s">
-        <v>7</v>
-      </c>
       <c r="F21" t="s">
         <v>7</v>
       </c>
-      <c r="G21">
+      <c r="G21" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21">
         <v>610</v>
       </c>
-      <c r="H21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
         <v>18</v>
       </c>
-      <c r="B22" t="s">
-        <v>17</v>
-      </c>
       <c r="C22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" t="s">
         <v>35</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>36</v>
       </c>
-      <c r="E22" t="s">
-        <v>7</v>
-      </c>
       <c r="F22" t="s">
         <v>7</v>
       </c>
-      <c r="G22">
+      <c r="G22" t="s">
+        <v>7</v>
+      </c>
+      <c r="H22">
         <v>610</v>
       </c>
-      <c r="H22" t="s">
-        <v>26</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>26</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="C23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" t="s">
         <v>33</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>37</v>
       </c>
-      <c r="E23" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23">
+      <c r="F23" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="H23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="C24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" t="s">
         <v>35</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>36</v>
       </c>
-      <c r="E24" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
+      <c r="F24" t="s">
+        <v>7</v>
       </c>
       <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="H24" t="s">
-        <v>26</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
+        <v>26</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" t="s">
         <v>33</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>37</v>
       </c>
-      <c r="E25" t="s">
-        <v>7</v>
-      </c>
-      <c r="H25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>7</v>
+      </c>
+      <c r="I25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" t="s">
         <v>35</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>36</v>
       </c>
-      <c r="E26" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
+      <c r="F26" t="s">
+        <v>7</v>
       </c>
       <c r="G26">
         <v>0</v>
       </c>
-      <c r="H26" t="s">
-        <v>26</v>
-      </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26" t="s">
+        <v>26</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" t="s">
         <v>33</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>37</v>
       </c>
-      <c r="E27" t="s">
-        <v>7</v>
-      </c>
-      <c r="H27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>7</v>
+      </c>
+      <c r="I27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" t="s">
         <v>35</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>36</v>
       </c>
-      <c r="E28" t="s">
-        <v>7</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
+      <c r="F28" t="s">
+        <v>7</v>
       </c>
       <c r="G28">
         <v>0</v>
       </c>
-      <c r="H28" t="s">
-        <v>26</v>
-      </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28" t="s">
+        <v>26</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" t="s">
         <v>33</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>37</v>
       </c>
-      <c r="E29" t="s">
-        <v>7</v>
-      </c>
-      <c r="H29" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>7</v>
+      </c>
+      <c r="I29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" t="s">
         <v>35</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>36</v>
       </c>
-      <c r="E30" t="s">
-        <v>7</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
+      <c r="F30" t="s">
+        <v>7</v>
       </c>
       <c r="G30">
         <v>0</v>
       </c>
-      <c r="H30" t="s">
-        <v>26</v>
-      </c>
-      <c r="I30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30" t="s">
+        <v>26</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" t="s">
         <v>33</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>37</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>23</v>
       </c>
-      <c r="H31" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>22</v>
       </c>
       <c r="B32" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" t="s">
         <v>35</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>36</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>23</v>
       </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
       <c r="G32">
         <v>0</v>
       </c>
-      <c r="H32" t="s">
-        <v>26</v>
-      </c>
-      <c r="I32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32" t="s">
+        <v>26</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>24</v>
       </c>
       <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" t="s">
         <v>25</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>33</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>37</v>
       </c>
-      <c r="E33" t="s">
-        <v>7</v>
-      </c>
-      <c r="H33">
+      <c r="F33" t="s">
+        <v>7</v>
+      </c>
+      <c r="I33">
         <v>600</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>24</v>
       </c>
       <c r="B34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" t="s">
         <v>25</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>35</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>36</v>
       </c>
-      <c r="E34" t="s">
-        <v>7</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
+      <c r="F34" t="s">
+        <v>7</v>
       </c>
       <c r="G34">
         <v>0</v>
       </c>
       <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
         <v>600</v>
       </c>
-      <c r="I34">
+      <c r="J34">
         <v>0</v>
       </c>
     </row>
@@ -1322,7 +1395,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Add missing NIFES columns (HCB + DDT)
</commit_message>
<xml_diff>
--- a/Input_data/Grenseverdier_fra_Sylvia.xlsx
+++ b/Input_data/Grenseverdier_fra_Sylvia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\seksjon 212\Contaminant_indicators\Input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1CD232-7CA7-4E23-AFE0-35EFB4861DDA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889880D6-A325-4BD0-BFFE-A92801620750}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22050" windowHeight="9540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="for R" sheetId="3" r:id="rId1"/>
     <sheet name="original" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="44">
   <si>
     <t>Miljøgift</t>
   </si>
@@ -518,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,19 +605,22 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
         <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H4">
-        <v>20</v>
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -625,19 +628,13 @@
         <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
       </c>
       <c r="I5">
-        <v>5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -645,33 +642,39 @@
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" t="s">
         <v>7</v>
       </c>
       <c r="I6">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" t="s">
         <v>7</v>
       </c>
       <c r="I7">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -679,19 +682,10 @@
         <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I8">
-        <v>30</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -699,27 +693,42 @@
         <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
+        <v>36</v>
       </c>
       <c r="I9">
-        <v>50</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+      <c r="H10">
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="I10">
-        <v>150</v>
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="J10" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -733,10 +742,16 @@
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
       </c>
       <c r="H11">
         <v>3.5000000000000001E-3</v>
@@ -750,31 +765,25 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H12">
-        <v>3.5000000000000001E-3</v>
+        <v>6.4999999999999997E-3</v>
       </c>
       <c r="I12">
-        <v>3.5000000000000001E-3</v>
+        <v>6.4999999999999997E-3</v>
       </c>
       <c r="J12" t="s">
         <v>31</v>
@@ -791,10 +800,16 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
       </c>
       <c r="H13">
         <v>6.4999999999999997E-3</v>
@@ -814,19 +829,16 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
+        <v>37</v>
+      </c>
+      <c r="F14" t="s">
+        <v>7</v>
       </c>
       <c r="H14">
         <v>6.4999999999999997E-3</v>
@@ -840,31 +852,22 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
         <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" t="s">
-        <v>7</v>
-      </c>
-      <c r="H15">
-        <v>6.4999999999999997E-3</v>
+        <v>34</v>
       </c>
       <c r="I15">
-        <v>6.4999999999999997E-3</v>
-      </c>
-      <c r="J15" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -878,13 +881,25 @@
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E16" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
       </c>
       <c r="I16">
         <v>75</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -895,39 +910,30 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E17" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
+        <v>37</v>
+      </c>
+      <c r="F17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" t="s">
+        <v>7</v>
       </c>
       <c r="I17">
-        <v>75</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
+        <v>200</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s">
         <v>33</v>
@@ -941,8 +947,11 @@
       <c r="G18" t="s">
         <v>7</v>
       </c>
-      <c r="I18">
-        <v>200</v>
+      <c r="H18">
+        <v>10</v>
+      </c>
+      <c r="I18" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -953,10 +962,10 @@
         <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F19" t="s">
         <v>7</v>
@@ -970,19 +979,25 @@
       <c r="I19" t="s">
         <v>26</v>
       </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>42</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
       </c>
       <c r="C20" t="s">
         <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F20" t="s">
         <v>7</v>
@@ -991,13 +1006,10 @@
         <v>7</v>
       </c>
       <c r="H20">
-        <v>10</v>
+        <v>610</v>
       </c>
       <c r="I20" t="s">
         <v>26</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1011,10 +1023,10 @@
         <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F21" t="s">
         <v>7</v>
@@ -1028,37 +1040,31 @@
       <c r="I21" t="s">
         <v>26</v>
       </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s">
         <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E22" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F22" t="s">
         <v>7</v>
       </c>
-      <c r="G22" t="s">
-        <v>7</v>
-      </c>
       <c r="H22">
-        <v>610</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="I22" t="s">
         <v>26</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1069,13 +1075,16 @@
         <v>17</v>
       </c>
       <c r="D23" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F23" t="s">
         <v>7</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
       </c>
       <c r="H23">
         <v>8.5000000000000006E-2</v>
@@ -1083,34 +1092,31 @@
       <c r="I23" t="s">
         <v>26</v>
       </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
+        <v>19</v>
       </c>
       <c r="C24" t="s">
         <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E24" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F24" t="s">
         <v>7</v>
       </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <v>8.5000000000000006E-2</v>
-      </c>
       <c r="I24" t="s">
         <v>26</v>
-      </c>
-      <c r="J24">
-        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1124,48 +1130,48 @@
         <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F25" t="s">
         <v>7</v>
       </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
       <c r="I25" t="s">
         <v>26</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C26" t="s">
         <v>17</v>
       </c>
       <c r="D26" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E26" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F26" t="s">
         <v>7</v>
       </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
       <c r="I26" t="s">
         <v>26</v>
-      </c>
-      <c r="J26">
-        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1179,48 +1185,48 @@
         <v>17</v>
       </c>
       <c r="D27" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F27" t="s">
         <v>7</v>
       </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
       <c r="I27" t="s">
         <v>26</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B28" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C28" t="s">
         <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E28" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F28" t="s">
         <v>7</v>
       </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
       <c r="I28" t="s">
         <v>26</v>
-      </c>
-      <c r="J28">
-        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1234,48 +1240,48 @@
         <v>17</v>
       </c>
       <c r="D29" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F29" t="s">
         <v>7</v>
       </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
       <c r="I29" t="s">
         <v>26</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C30" t="s">
         <v>17</v>
       </c>
       <c r="D30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E30" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F30" t="s">
-        <v>7</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I30" t="s">
         <v>26</v>
-      </c>
-      <c r="J30">
-        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -1289,48 +1295,48 @@
         <v>17</v>
       </c>
       <c r="D31" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F31" t="s">
         <v>23</v>
       </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
       <c r="I31" t="s">
         <v>26</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B32" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C32" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D32" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E32" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F32" t="s">
-        <v>23</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-      <c r="I32" t="s">
-        <v>26</v>
-      </c>
-      <c r="J32">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="I32">
+        <v>600</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -1344,47 +1350,24 @@
         <v>25</v>
       </c>
       <c r="D33" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F33" t="s">
         <v>7</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
       </c>
       <c r="I33">
         <v>600</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>24</v>
-      </c>
-      <c r="B34" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" t="s">
-        <v>25</v>
-      </c>
-      <c r="D34" t="s">
-        <v>35</v>
-      </c>
-      <c r="E34" t="s">
-        <v>36</v>
-      </c>
-      <c r="F34" t="s">
-        <v>7</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34">
-        <v>0</v>
-      </c>
-      <c r="I34">
-        <v>600</v>
-      </c>
-      <c r="J34">
+      <c r="J33">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Make new export file
- Building on updated BDES results for HI stations
- Also updated value limits (Grenseverdier
xlsx file) with Hg limits also for blue mussel
</commit_message>
<xml_diff>
--- a/Input_data/Grenseverdier_fra_Sylvia.xlsx
+++ b/Input_data/Grenseverdier_fra_Sylvia.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\seksjon 212\Contaminant_indicators\Input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889880D6-A325-4BD0-BFFE-A92801620750}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C01278-F034-43AC-AB3F-B5EBF9A90379}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22050" windowHeight="9540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="for R" sheetId="3" r:id="rId1"/>
     <sheet name="original" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027" iterateDelta="1E-4"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -521,7 +521,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="H3" sqref="H3:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,6 +601,12 @@
       </c>
       <c r="E3" t="s">
         <v>36</v>
+      </c>
+      <c r="H3">
+        <v>20</v>
+      </c>
+      <c r="I3">
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>